<commit_message>
juste changement de branche
</commit_message>
<xml_diff>
--- a/shéma de découpe.xlsx
+++ b/shéma de découpe.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre_Cuoq\Desktop\ClickerNSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CA7D559-C338-4AA3-A150-EDD0A4033813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C057E89-A4CA-4298-B437-019CDA2D5A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>Joueur : machin</t>
   </si>
@@ -72,12 +72,15 @@
   </si>
   <si>
     <t>explication</t>
+  </si>
+  <si>
+    <t>Bonus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -94,7 +97,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +134,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -302,102 +311,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -733,11 +730,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,20 +790,20 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="23"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="24"/>
+      <c r="M2" s="5"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -815,31 +812,31 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="23" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="25"/>
-      <c r="J3" s="20"/>
+      <c r="J3" s="24"/>
       <c r="K3" s="1"/>
       <c r="L3" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="33" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>12</v>
       </c>
       <c r="P3" s="1"/>
     </row>
@@ -847,50 +844,50 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="26"/>
-      <c r="J4" s="18"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="28"/>
       <c r="K4" s="1"/>
       <c r="L4" s="30"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="34"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="18"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="28"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="29" t="s">
+      <c r="L5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="27" t="s">
+      <c r="M5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="33" t="s">
+      <c r="O5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="P5" s="1"/>
@@ -899,46 +896,46 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="34"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="9"/>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="29" t="s">
+      <c r="L7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="27" t="s">
+      <c r="M7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="31" t="s">
+      <c r="N7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="33" t="s">
+      <c r="O7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="P7" s="1"/>
@@ -947,48 +944,48 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="34"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="9"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="10"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="29" t="s">
+      <c r="L9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N9" s="31" t="s">
+      <c r="N9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="O9" s="33" t="s">
+      <c r="O9" s="8" t="s">
         <v>11</v>
       </c>
       <c r="P9" s="1"/>
@@ -997,46 +994,46 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="34"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="9"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="29" t="s">
+      <c r="L11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="27" t="s">
+      <c r="M11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="31" t="s">
+      <c r="N11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="33" t="s">
+      <c r="O11" s="8" t="s">
         <v>11</v>
       </c>
       <c r="P11" s="1"/>
@@ -1045,48 +1042,48 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="34"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="9"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="4"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="16"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="29" t="s">
+      <c r="L13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="27" t="s">
+      <c r="M13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N13" s="31" t="s">
+      <c r="N13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="33" t="s">
+      <c r="O13" s="8" t="s">
         <v>11</v>
       </c>
       <c r="P13" s="1"/>
@@ -1101,14 +1098,14 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="7"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="22"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="34"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="9"/>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1116,19 +1113,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="23"/>
+      <c r="J15" s="4"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="24"/>
+      <c r="M15" s="5"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1145,21 +1142,26 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="23"/>
+      <c r="J16" s="4"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="24"/>
+      <c r="M16" s="5"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="B3:F13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H9:J10"/>
+    <mergeCell ref="H13:J14"/>
     <mergeCell ref="L13:L14"/>
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="O5:O6"/>
@@ -1176,16 +1178,11 @@
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="N7:N8"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="B3:F13"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H9:J10"/>
-    <mergeCell ref="H13:J14"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="L11:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>